<commit_message>
Using Excel's LEN() Functions
</commit_message>
<xml_diff>
--- a/Section 26: Working with Excel's Text Based Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 26: Working with Excel's Text Based Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 26: Working with Excel's Text Based Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C21144-4AC6-074F-83F0-DCDAC8660FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC57DBF-AA72-0948-B0E1-6F7753943C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14501,7 +14501,7 @@
   <dimension ref="A2:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -14560,8 +14560,12 @@
         <v>110</v>
       </c>
       <c r="G3" s="17" t="str">
-        <f>RIGHT(A3,2)</f>
+        <f>IF(H3 = 8, RIGHT(A3,2), RIGHT(A3,4))</f>
         <v>WW</v>
+      </c>
+      <c r="H3">
+        <f>LEN(A3)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14">
@@ -14584,8 +14588,12 @@
         <v>111</v>
       </c>
       <c r="G4" s="17" t="str">
-        <f>RIGHT(A4,2)</f>
+        <f t="shared" ref="G4:G26" si="0">IF(H4 = 8, RIGHT(A4,2), RIGHT(A4,4))</f>
         <v>WW</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H26" si="1">LEN(A4)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14">
@@ -14600,16 +14608,20 @@
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="17" t="str">
-        <f t="shared" ref="E5:E17" si="0">LEFT(A5,3)</f>
+        <f t="shared" ref="E5:E17" si="2">LEFT(A5,3)</f>
         <v>ACM</v>
       </c>
       <c r="F5" s="17" t="str">
-        <f t="shared" ref="F5:F17" si="1">MID(A5,4,3)</f>
+        <f t="shared" ref="F5:F17" si="3">MID(A5,4,3)</f>
         <v>150</v>
       </c>
       <c r="G5" s="17" t="str">
-        <f t="shared" ref="G5:G17" si="2">RIGHT(A5,2)</f>
+        <f t="shared" si="0"/>
         <v>WW</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14">
@@ -14624,16 +14636,20 @@
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F6" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>321</v>
+      </c>
+      <c r="G6" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>ACM</v>
-      </c>
-      <c r="F6" s="17" t="str">
+        <v>DP</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>321</v>
-      </c>
-      <c r="G6" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>DP</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14">
@@ -14648,16 +14664,20 @@
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F7" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>322</v>
+      </c>
+      <c r="G7" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>ACM</v>
-      </c>
-      <c r="F7" s="17" t="str">
+        <v>DP</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>322</v>
-      </c>
-      <c r="G7" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>DP</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14">
@@ -14672,16 +14692,20 @@
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F8" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>325</v>
+      </c>
+      <c r="G8" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>ACM</v>
-      </c>
-      <c r="F8" s="17" t="str">
+        <v>DP</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>325</v>
-      </c>
-      <c r="G8" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>DP</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14">
@@ -14696,16 +14720,20 @@
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F9" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>330</v>
+      </c>
+      <c r="G9" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>ACM</v>
-      </c>
-      <c r="F9" s="17" t="str">
+        <v>DP</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>330</v>
-      </c>
-      <c r="G9" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>DP</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14">
@@ -14720,16 +14748,20 @@
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F10" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="G10" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>ACM</v>
-      </c>
-      <c r="F10" s="17" t="str">
+        <v>DP</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>450</v>
-      </c>
-      <c r="G10" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>DP</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14">
@@ -14744,16 +14776,20 @@
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ACM</v>
+      </c>
+      <c r="F11" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>460</v>
+      </c>
+      <c r="G11" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>ACM</v>
-      </c>
-      <c r="F11" s="17" t="str">
+        <v>DP</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>460</v>
-      </c>
-      <c r="G11" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>DP</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14">
@@ -14768,16 +14804,20 @@
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F12" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>530</v>
+      </c>
+      <c r="G12" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>AST</v>
-      </c>
-      <c r="F12" s="17" t="str">
+        <v>OL</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
-        <v>530</v>
-      </c>
-      <c r="G12" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>OL</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14">
@@ -14792,16 +14832,20 @@
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F13" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>AST</v>
-      </c>
-      <c r="F13" s="17" t="str">
+        <v>TF</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="G13" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>TF</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14">
@@ -14816,16 +14860,20 @@
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F14" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>130</v>
+      </c>
+      <c r="G14" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>AST</v>
-      </c>
-      <c r="F14" s="17" t="str">
+        <v>OL</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-      <c r="G14" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>OL</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14">
@@ -14840,16 +14888,20 @@
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F15" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="G15" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>AST</v>
-      </c>
-      <c r="F15" s="17" t="str">
+        <v>OL</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="1"/>
-        <v>140</v>
-      </c>
-      <c r="G15" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>OL</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14">
@@ -14864,19 +14916,23 @@
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F16" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="G16" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>AST</v>
-      </c>
-      <c r="F16" s="17" t="str">
+        <v>GO</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="G16" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>GO</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14">
       <c r="A17" s="22" t="s">
         <v>209</v>
       </c>
@@ -14888,19 +14944,23 @@
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>AST</v>
+      </c>
+      <c r="F17" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>121</v>
+      </c>
+      <c r="G17" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>AST</v>
-      </c>
-      <c r="F17" s="17" t="str">
+        <v>BF</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="G17" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v>BF</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14">
       <c r="A18" s="22" t="s">
         <v>210</v>
       </c>
@@ -14911,11 +14971,24 @@
         <v>6.5</v>
       </c>
       <c r="D18" s="37"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" ht="14">
+      <c r="E18" s="17" t="str">
+        <f>LEFT(A18,3)</f>
+        <v>AST</v>
+      </c>
+      <c r="F18" s="17" t="str">
+        <f>MID(A18,4,3)</f>
+        <v>132</v>
+      </c>
+      <c r="G18" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>PS</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14">
       <c r="A19" s="22" t="s">
         <v>178</v>
       </c>
@@ -14926,11 +14999,24 @@
         <v>4.55</v>
       </c>
       <c r="D19" s="37"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" ht="14">
+      <c r="E19" s="17" t="str">
+        <f t="shared" ref="E19:E26" si="4">LEFT(A19,3)</f>
+        <v>AST</v>
+      </c>
+      <c r="F19" s="17" t="str">
+        <f t="shared" ref="F19:F26" si="5">MID(A19,4,3)</f>
+        <v>205</v>
+      </c>
+      <c r="G19" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>0995</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14">
       <c r="A20" s="22" t="s">
         <v>211</v>
       </c>
@@ -14941,11 +15027,24 @@
         <v>14.3</v>
       </c>
       <c r="D20" s="37"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" ht="14">
+      <c r="E20" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>BVR</v>
+      </c>
+      <c r="F20" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>590</v>
+      </c>
+      <c r="G20" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>WF</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14">
       <c r="A21" s="22" t="s">
         <v>212</v>
       </c>
@@ -14956,11 +15055,24 @@
         <v>13.81</v>
       </c>
       <c r="D21" s="37"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" ht="14">
+      <c r="E21" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>BVR</v>
+      </c>
+      <c r="F21" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>690</v>
+      </c>
+      <c r="G21" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>AF</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14">
       <c r="A22" s="22" t="s">
         <v>217</v>
       </c>
@@ -14971,11 +15083,24 @@
         <v>7.31</v>
       </c>
       <c r="D22" s="37"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" ht="14">
+      <c r="E22" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>TRA</v>
+      </c>
+      <c r="F22" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>203</v>
+      </c>
+      <c r="G22" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14">
       <c r="A23" s="22" t="s">
         <v>218</v>
       </c>
@@ -14986,11 +15111,24 @@
         <v>7.31</v>
       </c>
       <c r="D23" s="37"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" ht="14">
+      <c r="E23" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>TRA</v>
+      </c>
+      <c r="F23" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>205</v>
+      </c>
+      <c r="G23" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14">
       <c r="A24" s="22" t="s">
         <v>214</v>
       </c>
@@ -15001,11 +15139,24 @@
         <v>7.31</v>
       </c>
       <c r="D24" s="37"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" ht="14">
+      <c r="E24" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>TRA</v>
+      </c>
+      <c r="F24" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>207</v>
+      </c>
+      <c r="G24" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="14">
       <c r="A25" s="22" t="s">
         <v>215</v>
       </c>
@@ -15016,11 +15167,24 @@
         <v>7.64</v>
       </c>
       <c r="D25" s="37"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="14">
+      <c r="E25" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>TRA</v>
+      </c>
+      <c r="F25" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>310</v>
+      </c>
+      <c r="G25" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="14">
       <c r="A26" s="22" t="s">
         <v>216</v>
       </c>
@@ -15031,9 +15195,22 @@
         <v>6.14</v>
       </c>
       <c r="D26" s="37"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="E26" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v>TRA</v>
+      </c>
+      <c r="F26" s="17" t="str">
+        <f t="shared" si="5"/>
+        <v>610</v>
+      </c>
+      <c r="G26" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>OF</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Using Excel's SEARCH() Functions
</commit_message>
<xml_diff>
--- a/Section 26: Working with Excel's Text Based Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 26: Working with Excel's Text Based Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 26: Working with Excel's Text Based Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC57DBF-AA72-0948-B0E1-6F7753943C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B289998-EA6F-254B-8564-E56F7749552E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="16940" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -2921,8 +2921,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2947,25 +2947,65 @@
       <c r="A2" t="s">
         <v>243</v>
       </c>
+      <c r="B2" t="str">
+        <f>LEFT(A2,SEARCH(" ",A2))</f>
+        <v xml:space="preserve">Patrick </v>
+      </c>
+      <c r="C2" t="str">
+        <f>RIGHT(A2,LEN(A2)-SEARCH(" ",A2))</f>
+        <v>Marleau</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>244</v>
       </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B6" si="0">LEFT(A3,SEARCH(" ",A3))</f>
+        <v xml:space="preserve">Joe </v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C6" si="1">RIGHT(A3,LEN(A3)-SEARCH(" ",A3))</f>
+        <v>Thornton</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>245</v>
       </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Brent </v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>Burns</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>246</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Joe </v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavelski</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>247</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Martin </v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>Jones</v>
       </c>
     </row>
   </sheetData>
@@ -14500,7 +14540,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Using Excel's CONCATENTATE() Functions
</commit_message>
<xml_diff>
--- a/Section 26: Working with Excel's Text Based Functions/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 26: Working with Excel's Text Based Functions/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 26: Working with Excel's Text Based Functions/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B289998-EA6F-254B-8564-E56F7749552E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F855C15-2BD9-4B41-A605-CA8B7F326903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="16940" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16960" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -2921,7 +2921,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
@@ -3019,8 +3019,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -3063,7 +3063,10 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
+      <c r="E4" s="131" t="str">
+        <f>_xlfn.CONCAT(C4, " ", B4)</f>
+        <v>Joe Gonzales</v>
+      </c>
       <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="14">
@@ -3073,7 +3076,10 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
+      <c r="E5" s="131" t="str">
+        <f t="shared" ref="E5:E17" si="0">_xlfn.CONCAT(C5, " ", B5)</f>
+        <v>Gail Scote</v>
+      </c>
       <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="14">
@@ -3083,7 +3089,10 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
+      <c r="E6" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Sheryl Kane</v>
+      </c>
       <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="14">
@@ -3093,7 +3102,10 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
+      <c r="E7" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Kendrick Hapsbuch</v>
+      </c>
       <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="14">
@@ -3103,7 +3115,10 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
+      <c r="E8" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Henders</v>
+      </c>
       <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="14">
@@ -3113,7 +3128,10 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
+      <c r="E9" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Katie Atherton</v>
+      </c>
       <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="14">
@@ -3123,7 +3141,10 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
+      <c r="E10" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Frank Bellwood</v>
+      </c>
       <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="14">
@@ -3133,7 +3154,10 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
+      <c r="E11" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Linda Cooper</v>
+      </c>
       <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="14">
@@ -3143,7 +3167,10 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
+      <c r="E12" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Brent Cronwith</v>
+      </c>
       <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="14">
@@ -3153,7 +3180,10 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
+      <c r="E13" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Sandrae Simpson</v>
+      </c>
       <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="14">
@@ -3163,7 +3193,10 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
+      <c r="E14" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Randy Sindole</v>
+      </c>
       <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="14">
@@ -3173,7 +3206,10 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
+      <c r="E15" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Ellen Smith</v>
+      </c>
       <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="14">
@@ -3183,7 +3219,10 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
+      <c r="E16" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuome Vuanuo</v>
+      </c>
       <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="14">
@@ -3193,7 +3232,10 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
+      <c r="E17" s="131" t="str">
+        <f t="shared" si="0"/>
+        <v>Tadeuz Szcznyck</v>
+      </c>
       <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="14">
@@ -3203,7 +3245,10 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
+      <c r="E18" s="131" t="str">
+        <f>_xlfn.CONCAT(C18, " ", B18)</f>
+        <v>Tammy Wu</v>
+      </c>
       <c r="F18" s="132"/>
     </row>
   </sheetData>

</xml_diff>